<commit_message>
excel with total and subtotal
</commit_message>
<xml_diff>
--- a/several_pages.xlsx
+++ b/several_pages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
   <si>
     <t>វិក្កយប័ត្រអាករ</t>
   </si>
@@ -215,6 +215,63 @@
   </si>
   <si>
     <t>272.73</t>
+  </si>
+  <si>
+    <t>សរុប</t>
+  </si>
+  <si>
+    <t>Total  :</t>
+  </si>
+  <si>
+    <t>1,467.27</t>
+  </si>
+  <si>
+    <t>អាករលើតម្លែបន្ថែម ១០%</t>
+  </si>
+  <si>
+    <t>VAT 10%:</t>
+  </si>
+  <si>
+    <t>សរុបរួម</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL:</t>
+  </si>
+  <si>
+    <t>1,614.00</t>
+  </si>
+  <si>
+    <t>ការទូទាត់អាចធ្វើឡើងតាមមូលឡបទានប័ត្រ</t>
+  </si>
+  <si>
+    <t>ហត្ថលេខា</t>
+  </si>
+  <si>
+    <t>ឬ តាមរយ:ការទូទាត់ទៅធនាគារ</t>
+  </si>
+  <si>
+    <t>Authorized Signature</t>
+  </si>
+  <si>
+    <t>Payment can be made by Cheque</t>
+  </si>
+  <si>
+    <t>or Bank Transfer payable to :</t>
+  </si>
+  <si>
+    <t>Account Name: Cambodian Broadcasting Service</t>
+  </si>
+  <si>
+    <t>-------------------------------</t>
+  </si>
+  <si>
+    <t>Account No  : USD 116345</t>
+  </si>
+  <si>
+    <t>Bank Name   : ANZ Royal Bank (Cambodia) Ltd</t>
+  </si>
+  <si>
+    <t>SWIFT CODE: ANZBKHPP</t>
   </si>
 </sst>
 </file>
@@ -613,7 +670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I37"/>
+  <dimension ref="B1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17355,56 +17412,138 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" t="s" s="3">
-        <v>35</v>
+    <row r="47" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F47" t="s" s="2">
+        <v>67</v>
       </c>
-      <c r="C34" t="s" s="3">
-        <v>35</v>
+      <c r="G47" t="s" s="2">
+        <v>68</v>
       </c>
-      <c r="D34" t="s" s="3">
-        <v>35</v>
+      <c r="I47" t="s" s="2">
+        <v>69</v>
       </c>
-      <c r="E34" t="s" s="3">
-        <v>35</v>
+    </row>
+    <row r="48" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F48" t="s" s="2">
+        <v>70</v>
       </c>
-      <c r="F34" t="s" s="3">
-        <v>35</v>
+      <c r="G48" t="s" s="2">
+        <v>71</v>
       </c>
-      <c r="G34" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="H34" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="I34" t="s" s="3">
+      <c r="I48" t="s" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" t="s" s="3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="C37" t="s" s="3">
+      <c r="C50" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="D37" t="s" s="3">
+      <c r="D50" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="E37" t="s" s="3">
+      <c r="E50" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="F37" t="s" s="3">
+      <c r="F50" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="G37" t="s" s="3">
+      <c r="G50" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="H37" t="s" s="3">
+      <c r="H50" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="I37" t="s" s="3">
+      <c r="I50" t="s" s="3">
         <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F51" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="G51" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I51" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="D53" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="E53" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="F53" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="G53" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="H53" t="s" s="3">
+        <v>35</v>
+      </c>
+      <c r="I53" t="s" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s" s="2">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>